<commit_message>
WE FORGOT RANGE :(
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22538DB2-68EF-4536-A0C7-0D86B2DA01AF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73090F-3CCB-4EF1-9504-059E46E1EC88}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
@@ -510,34 +510,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0.59330543933054392</v>
+        <v>1.231902869808319</v>
       </c>
       <c r="E2">
-        <v>0.21666666666666667</v>
+        <v>0.29273040859629668</v>
       </c>
       <c r="F2">
-        <v>0.73400383141762437</v>
+        <v>1.5385714285714283</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>342</v>
       </c>
       <c r="H2">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I2">
-        <v>112</v>
+        <v>412</v>
       </c>
       <c r="J2">
-        <v>1036</v>
+        <v>1097</v>
       </c>
       <c r="K2">
-        <v>127</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -580,16 +580,16 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>0.29375000000000007</v>
+        <v>0.45333333333333325</v>
       </c>
       <c r="E2">
-        <v>0.21309523809523817</v>
+        <v>0.43981481481481466</v>
       </c>
       <c r="F2">
-        <v>0.85833333333333328</v>
+        <v>0.57500000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,19 +597,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.37575757575757573</v>
+        <v>1.221759259259259</v>
       </c>
       <c r="E3">
-        <v>0.19583333333333341</v>
+        <v>0.26851851851851838</v>
       </c>
       <c r="F3">
-        <v>0.41574074074074063</v>
+        <v>1.5395061728395061</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -617,19 +617,19 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.33492063492063484</v>
+        <v>0.66896551724137943</v>
       </c>
       <c r="E4">
-        <v>0.29333333333333333</v>
+        <v>0.2777777777777779</v>
       </c>
       <c r="F4">
-        <v>0.34791666666666654</v>
+        <v>0.84500000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -637,19 +637,19 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.29649122807017547</v>
+        <v>1.9944444444444445</v>
       </c>
       <c r="E5">
-        <v>0.18571428571428572</v>
+        <v>0.3</v>
       </c>
       <c r="F5">
-        <v>0.36111111111111116</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -657,19 +657,19 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.48541666666666655</v>
+        <v>0.3520833333333333</v>
       </c>
       <c r="E6">
-        <v>0.17222222222222192</v>
+        <v>0.15555555555555545</v>
       </c>
       <c r="F6">
-        <v>0.5576923076923076</v>
+        <v>0.47000000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,19 +677,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.77894736842105272</v>
+        <v>1.1746666666666667</v>
       </c>
       <c r="E7">
-        <v>0.20833333333333326</v>
+        <v>0.11666666666666625</v>
       </c>
       <c r="F7">
-        <v>0.84607843137254923</v>
+        <v>1.3761904761904762</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,19 +697,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.50526315789473697</v>
+        <v>1.6672222222222222</v>
       </c>
       <c r="E8">
-        <v>0.19666666666666671</v>
+        <v>0.16111111111111118</v>
       </c>
       <c r="F8">
-        <v>0.61547619047619051</v>
+        <v>2.0437499999999997</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,19 +717,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.64924242424242407</v>
+        <v>1.1446666666666667</v>
       </c>
       <c r="E9">
-        <v>0.16666666666666641</v>
+        <v>0.13888888888888865</v>
       </c>
       <c r="F9">
-        <v>0.6974999999999999</v>
+        <v>1.281818181818182</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -737,19 +737,19 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>1.199242424242424</v>
+        <v>2.4153846153846148</v>
       </c>
       <c r="E10">
-        <v>0.32777777777777778</v>
+        <v>0.48095238095238096</v>
       </c>
       <c r="F10">
-        <v>1.5260416666666663</v>
+        <v>3.1280701754385958</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -757,19 +757,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1.6031249999999999</v>
+        <v>2.5348484848484856</v>
       </c>
       <c r="E11">
-        <v>0.18888888888888911</v>
+        <v>0.46666666666666656</v>
       </c>
       <c r="F11">
-        <v>1.9294871794871793</v>
+        <v>2.741666666666668</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,19 +777,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.28437500000000016</v>
+        <v>0.29393939393939378</v>
       </c>
       <c r="E12">
-        <v>0.16666666666666696</v>
+        <v>0.10555555555555533</v>
       </c>
       <c r="F12">
-        <v>0.33787878787878795</v>
+        <v>0.32368421052631569</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -797,19 +797,19 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.65641025641025652</v>
+        <v>1.5356060606060604</v>
       </c>
       <c r="E13">
-        <v>0.29999999999999982</v>
+        <v>0.34999999999999964</v>
       </c>
       <c r="F13">
-        <v>0.68611111111111123</v>
+        <v>1.6541666666666668</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -817,19 +817,19 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.25555555555555554</v>
+        <v>0.64679487179487194</v>
       </c>
       <c r="E14">
-        <v>0.2041666666666665</v>
+        <v>0.23666666666666664</v>
       </c>
       <c r="F14">
-        <v>0.29666666666666675</v>
+        <v>0.74444444444444458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved work to update main files
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABB329C-0E0B-4D5D-88D3-E4E46BC78172}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A048EC-DE44-4957-92B9-B33AB1C50BA2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
@@ -510,34 +510,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>2.6865879767113823</v>
+        <v>1.9521901716272532</v>
       </c>
       <c r="E2">
-        <v>0.46767390830041622</v>
+        <v>0.26785244902410543</v>
       </c>
       <c r="F2">
-        <v>3.6449921752738654</v>
+        <v>2.6585253456221216</v>
       </c>
       <c r="G2">
-        <v>147</v>
+        <v>287</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="I2">
-        <v>182</v>
+        <v>360</v>
       </c>
       <c r="J2">
-        <v>589</v>
+        <v>1138</v>
       </c>
       <c r="K2">
-        <v>62</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +577,19 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1.4293333333333336</v>
+        <v>0.93275862068965509</v>
       </c>
       <c r="E2">
-        <v>0.66333333333333355</v>
+        <v>0.25289855072463768</v>
       </c>
       <c r="F2">
-        <v>4.4933333333333341</v>
+        <v>3.5388888888888883</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,19 +597,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2.2993055555555557</v>
+        <v>2.0765151515151516</v>
       </c>
       <c r="E3">
-        <v>0.43181818181818171</v>
+        <v>0.4166666666666668</v>
       </c>
       <c r="F3">
-        <v>3.8794871794871799</v>
+        <v>2.4453703703703709</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -617,19 +617,19 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>2.9666666666666668</v>
+        <v>1.7222222222222221</v>
       </c>
       <c r="E4">
-        <v>0.50000000000000011</v>
+        <v>0.23333333333333328</v>
       </c>
       <c r="F4">
-        <v>3.5833333333333335</v>
+        <v>2.2636363636363637</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -637,19 +637,19 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2.7729166666666658</v>
+        <v>2.2646666666666664</v>
       </c>
       <c r="E5">
-        <v>0.65666666666666651</v>
+        <v>0.27333333333333359</v>
       </c>
       <c r="F5">
-        <v>3.329824561403508</v>
+        <v>2.7624999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -657,19 +657,19 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>2.5938271604938277</v>
+        <v>1.0075757575757578</v>
       </c>
       <c r="E6">
-        <v>0.25277777777777777</v>
+        <v>0.1499999999999998</v>
       </c>
       <c r="F6">
-        <v>3.2626984126984135</v>
+        <v>1.2598039215686276</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,19 +677,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>2.5654320987654327</v>
+        <v>1.3674242424242424</v>
       </c>
       <c r="E7">
-        <v>0.29999999999999971</v>
+        <v>0.21333333333333329</v>
       </c>
       <c r="F7">
-        <v>3.6981481481481486</v>
+        <v>1.7068627450980394</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,19 +697,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>2.9580246913580259</v>
+        <v>2.6716666666666669</v>
       </c>
       <c r="E8">
-        <v>0.24166666666666681</v>
+        <v>0.26000000000000006</v>
       </c>
       <c r="F8">
-        <v>3.4304347826086969</v>
+        <v>3.4755555555555562</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,19 +717,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>2.0256410256410255</v>
+        <v>2.4746031746031738</v>
       </c>
       <c r="E9">
-        <v>0.37777777777777766</v>
+        <v>0.23666666666666672</v>
       </c>
       <c r="F9">
-        <v>2.8980392156862744</v>
+        <v>3.1739583333333328</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -737,19 +737,19 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10">
-        <v>3.5149122807017541</v>
+        <v>3.4172839506172838</v>
       </c>
       <c r="E10">
-        <v>0.59333333333333338</v>
+        <v>0.45208333333333361</v>
       </c>
       <c r="F10">
-        <v>4.5583333333333336</v>
+        <v>4.6657894736842103</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -757,19 +757,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1.6633333333333333</v>
+        <v>3.0320000000000009</v>
       </c>
       <c r="E11">
-        <v>0.36333333333333323</v>
+        <v>0.28750000000000003</v>
       </c>
       <c r="F11">
-        <v>2.9633333333333334</v>
+        <v>3.5547619047619059</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,19 +777,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>3.5105263157894737</v>
+        <v>1.138095238095238</v>
       </c>
       <c r="E12">
-        <v>0.26111111111111091</v>
+        <v>0.14666666666666678</v>
       </c>
       <c r="F12">
-        <v>4.119791666666667</v>
+        <v>1.4479166666666665</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -797,19 +797,19 @@
         <v>23</v>
       </c>
       <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
       <c r="D13">
-        <v>2.8982142857142863</v>
+        <v>1.1291666666666662</v>
       </c>
       <c r="E13">
-        <v>0.61190476190476206</v>
+        <v>0.36166666666666653</v>
       </c>
       <c r="F13">
-        <v>3.6603174603174615</v>
+        <v>1.6773809523809518</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -817,19 +817,19 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>3.4413793103448267</v>
+        <v>1.9842857142857144</v>
       </c>
       <c r="E14">
-        <v>0.3958333333333332</v>
+        <v>0.15625000000000003</v>
       </c>
       <c r="F14">
-        <v>3.9286666666666656</v>
+        <v>2.5259259259259261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 different versions, about to try continuous priority values.
Version 4 (UAV4, Req4,RZ4,Manager4, Master 1, Sim1)-Single Cargo type
Version 5 (UAV5,Req5,...Master/Sim 2) - H and L cargo
Version 6 (UAV6,Req6,... Master/Sim 3) - Continuous probability, 2 cargo categories
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E3D30-6392-4BF8-AF14-7F7C07BEFDCA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70F03F-23CC-4711-8082-ADE1D860E57B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
@@ -510,34 +510,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.4384636052956208</v>
+        <v>1.7747296719856605</v>
       </c>
       <c r="E2">
-        <v>0.44925239779400566</v>
+        <v>0.33739693645722207</v>
       </c>
       <c r="F2">
-        <v>3.0796143250688686</v>
+        <v>2.4003921568627455</v>
       </c>
       <c r="G2">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H2">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="I2">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="J2">
-        <v>353</v>
+        <v>575</v>
       </c>
       <c r="K2">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +577,19 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>2.260416666666667</v>
+        <v>0.51999999999999991</v>
       </c>
       <c r="E2">
-        <v>0.54629629629629639</v>
+        <v>0.54074074074074074</v>
       </c>
       <c r="F2">
-        <v>4.4642857142857144</v>
+        <v>0.33333333333333326</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,19 +597,16 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.6392857142857147</v>
-      </c>
-      <c r="E3">
-        <v>0.64444444444444438</v>
+        <v>1.6261904761904762</v>
       </c>
       <c r="F3">
-        <v>3.183333333333334</v>
+        <v>1.6261904761904762</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -617,19 +614,19 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2.7622222222222224</v>
+        <v>2.6777777777777776</v>
       </c>
       <c r="E4">
-        <v>0.39999999999999997</v>
+        <v>0.28333333333333321</v>
       </c>
       <c r="F4">
-        <v>3.3527777777777779</v>
+        <v>3.3619047619047615</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -637,19 +634,19 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2.4448717948717951</v>
+        <v>1.6041666666666661</v>
       </c>
       <c r="E5">
-        <v>0.36111111111111116</v>
+        <v>0.21666666666666648</v>
       </c>
       <c r="F5">
-        <v>3.0700000000000003</v>
+        <v>2.4366666666666661</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -663,13 +660,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.8385416666666667</v>
+        <v>2.0944444444444446</v>
       </c>
       <c r="E6">
-        <v>8.3333333333333259E-2</v>
+        <v>0.26111111111111107</v>
       </c>
       <c r="F6">
-        <v>1.9555555555555557</v>
+        <v>3.0111111111111115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,19 +674,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.73666666666666669</v>
+        <v>1.7708333333333333</v>
       </c>
       <c r="E7">
-        <v>0.31666666666666671</v>
+        <v>0.21666666666666679</v>
       </c>
       <c r="F7">
-        <v>0.91666666666666674</v>
+        <v>1.9928571428571427</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,19 +694,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>3.2280303030303044</v>
+        <v>2.3576923076923082</v>
       </c>
       <c r="E8">
-        <v>0.53333333333333333</v>
+        <v>0.26666666666666672</v>
       </c>
       <c r="F8">
-        <v>3.8268518518518531</v>
+        <v>3.2870370370370376</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,19 +714,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>2.2333333333333334</v>
+        <v>1.3222222222222226</v>
       </c>
       <c r="E9">
-        <v>0.39999999999999991</v>
+        <v>0.22333333333333333</v>
       </c>
       <c r="F9">
-        <v>4.0666666666666664</v>
+        <v>2.1071428571428577</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -737,16 +734,19 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>4.4750000000000005</v>
+        <v>1.2194444444444443</v>
+      </c>
+      <c r="E10">
+        <v>0.66666666666666674</v>
       </c>
       <c r="F10">
-        <v>4.4750000000000005</v>
+        <v>1.4958333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,19 +754,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3.1759259259259256</v>
+        <v>2.9999999999999991</v>
       </c>
       <c r="E11">
-        <v>0.19166666666666674</v>
+        <v>0.1416666666666665</v>
       </c>
       <c r="F11">
-        <v>4.0285714285714285</v>
+        <v>3.5196969696969687</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -774,19 +774,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1.8952380952380954</v>
+        <v>0.95784313725490189</v>
       </c>
       <c r="E12">
-        <v>0.18333333333333346</v>
+        <v>0.23999999999999982</v>
       </c>
       <c r="F12">
-        <v>2.58</v>
+        <v>1.2569444444444444</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,19 +794,19 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1.3606060606060604</v>
+        <v>1.3729166666666668</v>
       </c>
       <c r="E13">
-        <v>0.62777777777777755</v>
+        <v>0.41666666666666696</v>
       </c>
       <c r="F13">
-        <v>1.6354166666666665</v>
+        <v>1.5095238095238095</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -814,19 +814,16 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2.5568627450980395</v>
-      </c>
-      <c r="E14">
-        <v>0.45833333333333304</v>
+        <v>4.95</v>
       </c>
       <c r="F14">
-        <v>3.2025641025641032</v>
+        <v>4.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generalized time and priority factors
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E01DE-8D15-4013-81E0-475B6F8793DD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56E45F4-CD7D-4286-91A4-C2D9A66F8125}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
@@ -510,34 +510,34 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>1.1072865120067301</v>
+      </c>
+      <c r="E2">
+        <v>0.55175438596491255</v>
+      </c>
+      <c r="F2">
+        <v>1.3102694042143173</v>
+      </c>
+      <c r="G2">
         <v>42</v>
       </c>
-      <c r="D2">
-        <v>2.0448479632942234</v>
-      </c>
-      <c r="E2">
-        <v>0.51111111111111118</v>
-      </c>
-      <c r="F2">
-        <v>2.1078782448907898</v>
-      </c>
-      <c r="G2">
-        <v>41</v>
-      </c>
       <c r="H2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I2">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J2">
-        <v>317</v>
+        <v>537</v>
       </c>
       <c r="K2">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -577,16 +577,19 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>2.4020833333333336</v>
+        <v>0.98666666666666691</v>
+      </c>
+      <c r="E2">
+        <v>0.23333333333333339</v>
       </c>
       <c r="F2">
-        <v>2.4020833333333336</v>
+        <v>1.0404761904761908</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -594,16 +597,16 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>2.8958333333333335</v>
+        <v>1.8404761904761904</v>
       </c>
       <c r="F3">
-        <v>2.8958333333333335</v>
+        <v>1.8404761904761904</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -611,19 +614,19 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>2.3833333333333333</v>
+        <v>1.6714285714285713</v>
       </c>
       <c r="E4">
-        <v>1.2333333333333332</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="F4">
-        <v>2.5270833333333331</v>
+        <v>1.9545454545454546</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -631,19 +634,19 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1.4999999999999998</v>
+        <v>0.82222222222222197</v>
       </c>
       <c r="E5">
-        <v>0.38333333333333375</v>
+        <v>0.33333333333333348</v>
       </c>
       <c r="F5">
-        <v>1.6116666666666664</v>
+        <v>0.91999999999999971</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -651,16 +654,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>2.7363636363636363</v>
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="E6">
+        <v>0.50833333333333375</v>
       </c>
       <c r="F6">
-        <v>2.7363636363636363</v>
+        <v>0.49999999999999956</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -668,16 +674,19 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1.0023809523809526</v>
+        <v>0.67395833333333344</v>
+      </c>
+      <c r="E7">
+        <v>0.45714285714285724</v>
       </c>
       <c r="F7">
-        <v>1.0023809523809526</v>
+        <v>0.84259259259259267</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -685,19 +694,19 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>2.0430555555555556</v>
+        <v>0.63000000000000012</v>
       </c>
       <c r="E8">
-        <v>0.14999999999999997</v>
+        <v>0.41333333333333344</v>
       </c>
       <c r="F8">
-        <v>2.2151515151515153</v>
+        <v>0.84666666666666668</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -705,19 +714,19 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
-        <v>1.7287878787878783</v>
+        <v>0.43958333333333333</v>
       </c>
       <c r="E9">
-        <v>0.33333333333333348</v>
+        <v>0.38333333333333341</v>
       </c>
       <c r="F9">
-        <v>1.868333333333333</v>
+        <v>0.45833333333333326</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -725,16 +734,16 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>2.9009803921568635</v>
+        <v>1.6621212121212119</v>
       </c>
       <c r="F10">
-        <v>2.9009803921568635</v>
+        <v>1.6621212121212119</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -745,16 +754,16 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>1.1366666666666667</v>
+        <v>1.4051282051282052</v>
       </c>
       <c r="E11">
-        <v>0.64999999999999991</v>
+        <v>1.6944444444444444</v>
       </c>
       <c r="F11">
-        <v>1.1907407407407407</v>
+        <v>1.3183333333333336</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -762,16 +771,19 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1.0857142857142859</v>
+        <v>0.3708333333333334</v>
+      </c>
+      <c r="E12">
+        <v>0.38333333333333336</v>
       </c>
       <c r="F12">
-        <v>1.0857142857142859</v>
+        <v>0.33333333333333348</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -779,19 +791,19 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>2.1333333333333333</v>
+        <v>1.2013888888888891</v>
       </c>
       <c r="E13">
-        <v>0.31666666666666665</v>
+        <v>0.61333333333333351</v>
       </c>
       <c r="F13">
-        <v>2.3149999999999999</v>
+        <v>1.6214285714285717</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -799,16 +811,19 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>2.1055555555555556</v>
+        <v>1.3870370370370371</v>
+      </c>
+      <c r="E14">
+        <v>0.33333333333333331</v>
       </c>
       <c r="F14">
-        <v>2.1055555555555556</v>
+        <v>1.597777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a cargo bug
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22985677-F4D6-456C-A40B-244F97CCC1EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D984F0-CB2B-4A6F-984F-6AC37FC4F0E7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
@@ -510,34 +510,34 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>1.2181821527958214</v>
+        <v>0.6527948839311194</v>
       </c>
       <c r="E2">
-        <v>0.54491525423728804</v>
+        <v>0.51851851851851849</v>
       </c>
       <c r="F2">
-        <v>1.5929250491633071</v>
+        <v>0.8087287276360754</v>
       </c>
       <c r="G2">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="H2">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="J2">
-        <v>778</v>
+        <v>346</v>
       </c>
       <c r="K2">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +577,19 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1.1538461538461535</v>
+        <v>0.65999999999999992</v>
       </c>
       <c r="E2">
-        <v>0.91999999999999937</v>
+        <v>0.4444444444444442</v>
       </c>
       <c r="F2">
-        <v>1.2999999999999998</v>
+        <v>0.98333333333333361</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,19 +597,19 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1.3750000000000002</v>
+        <v>0.71875</v>
       </c>
       <c r="E3">
-        <v>0.82083333333333364</v>
+        <v>0.82777777777777783</v>
       </c>
       <c r="F3">
-        <v>1.5597222222222225</v>
+        <v>0.65333333333333321</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -617,19 +617,19 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>1.4453703703703706</v>
+        <v>0.52619047619047621</v>
       </c>
       <c r="E4">
-        <v>0.29666666666666675</v>
+        <v>0.68333333333333313</v>
       </c>
       <c r="F4">
-        <v>1.8871794871794876</v>
+        <v>0.46333333333333349</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -637,19 +637,19 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.91025641025641046</v>
+        <v>0.80833333333333324</v>
       </c>
       <c r="E5">
-        <v>0.58333333333333337</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="F5">
-        <v>1.0555555555555558</v>
+        <v>0.59166666666666656</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -657,19 +657,16 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.44861111111111091</v>
+        <v>0.41212121212121217</v>
       </c>
       <c r="E6">
-        <v>0.29166666666666663</v>
-      </c>
-      <c r="F6">
-        <v>1.2333333333333325</v>
+        <v>0.41212121212121217</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,19 +674,19 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.94393939393939386</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="E7">
-        <v>0.24333333333333335</v>
+        <v>0.24999999999999994</v>
       </c>
       <c r="F7">
-        <v>1.5277777777777777</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,19 +694,19 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1.4138888888888888</v>
+        <v>0.48333333333333323</v>
       </c>
       <c r="E8">
-        <v>0.44722222222222219</v>
+        <v>0.44166666666666649</v>
       </c>
       <c r="F8">
-        <v>2.3805555555555555</v>
+        <v>0.56666666666666687</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,19 +714,19 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1.55</v>
+        <v>0.71111111111111103</v>
       </c>
       <c r="E9">
-        <v>1.2066666666666668</v>
+        <v>0.65666666666666662</v>
       </c>
       <c r="F9">
-        <v>1.8933333333333331</v>
+        <v>0.77916666666666656</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -737,16 +734,16 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>1.5933333333333333</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="F10">
-        <v>1.5933333333333333</v>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,19 +751,19 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>0.90476190476190455</v>
+        <v>0.8</v>
       </c>
       <c r="E11">
-        <v>0.7277777777777773</v>
+        <v>0.25000000000000011</v>
       </c>
       <c r="F11">
-        <v>1.0375000000000001</v>
+        <v>1.1666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -774,19 +771,16 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.68749999999999967</v>
+        <v>0.37222222222222218</v>
       </c>
       <c r="E12">
-        <v>0.33958333333333302</v>
-      </c>
-      <c r="F12">
-        <v>1.3833333333333331</v>
+        <v>0.37222222222222218</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,19 +788,16 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>1.2616666666666669</v>
-      </c>
-      <c r="E13">
-        <v>0.67500000000000004</v>
+        <v>1.1138888888888892</v>
       </c>
       <c r="F13">
-        <v>1.4083333333333337</v>
+        <v>1.1138888888888892</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -814,16 +805,16 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1.9083333333333332</v>
-      </c>
-      <c r="F14">
-        <v>1.9083333333333332</v>
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="E14">
+        <v>0.6166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tests to run 30 trials
</commit_message>
<xml_diff>
--- a/Current_Workspace/singleRun.xlsx
+++ b/Current_Workspace/singleRun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Current_Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280A00F5-F93C-4E99-A773-A110D36A5D7C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD253232-5F7A-4F67-AE66-F10F6C4B198A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11352" windowHeight="11220" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
+    <workbookView xWindow="4164" yWindow="672" windowWidth="9168" windowHeight="8964" activeTab="2" xr2:uid="{561E10B6-D33F-49E5-B70C-F7C1FE532749}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,34 +510,34 @@
         <v>8</v>
       </c>
       <c r="B2">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="D2">
+        <v>1.351266104806558</v>
+      </c>
+      <c r="E2">
+        <v>0.52222222222222203</v>
+      </c>
+      <c r="F2">
+        <v>1.5675384220024717</v>
+      </c>
+      <c r="G2">
+        <v>62</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2">
         <v>102</v>
       </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>1.5334824863578203</v>
-      </c>
-      <c r="E2">
-        <v>0.64</v>
-      </c>
-      <c r="F2">
-        <v>1.6741883897212564</v>
-      </c>
-      <c r="G2">
-        <v>60</v>
-      </c>
-      <c r="H2">
-        <v>43</v>
-      </c>
-      <c r="I2">
-        <v>103</v>
-      </c>
       <c r="J2">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="K2">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +577,19 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1.8499999999999996</v>
+        <v>1.0089743589743587</v>
       </c>
       <c r="E2">
-        <v>1.3166666666666667</v>
+        <v>0.26666666666666661</v>
       </c>
       <c r="F2">
-        <v>2.3833333333333329</v>
+        <v>1.0708333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,19 +597,19 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.9020833333333336</v>
+        <v>0.85277777777777775</v>
       </c>
       <c r="E3">
-        <v>0.58333333333333326</v>
+        <v>0.39999999999999974</v>
       </c>
       <c r="F3">
-        <v>2.0904761904761906</v>
+        <v>1.3055555555555556</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -617,19 +617,19 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1.7833333333333332</v>
+        <v>0.99750000000000016</v>
       </c>
       <c r="E4">
-        <v>0.3833333333333333</v>
+        <v>0.43333333333333313</v>
       </c>
       <c r="F4">
-        <v>1.8708333333333333</v>
+        <v>1.1385416666666668</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -637,19 +637,19 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>1.4333333333333336</v>
+        <v>1.8766666666666665</v>
       </c>
       <c r="E5">
-        <v>0.2833333333333341</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="F5">
-        <v>1.6633333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -657,19 +657,19 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1.5192307692307692</v>
+        <v>1.4033333333333335</v>
       </c>
       <c r="E6">
-        <v>0.61666666666666536</v>
+        <v>0.86666666666666625</v>
       </c>
       <c r="F6">
-        <v>1.5944444444444443</v>
+        <v>1.462962962962963</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -677,16 +677,19 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>2.0772727272727276</v>
+        <v>1.9769230769230766</v>
+      </c>
+      <c r="E7">
+        <v>0.43749999999999956</v>
       </c>
       <c r="F7">
-        <v>2.0772727272727276</v>
+        <v>2.661111111111111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -694,19 +697,19 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1.0833333333333333</v>
+        <v>0.61111111111111072</v>
       </c>
       <c r="E8">
-        <v>0.21666666666666676</v>
+        <v>0.4833333333333325</v>
       </c>
       <c r="F8">
-        <v>1.3722222222222222</v>
+        <v>0.86666666666666714</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -714,19 +717,16 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.3794871794871795</v>
-      </c>
-      <c r="E9">
-        <v>0.29999999999999982</v>
+        <v>2.1071428571428572</v>
       </c>
       <c r="F9">
-        <v>1.4694444444444443</v>
+        <v>2.1071428571428572</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -734,19 +734,19 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>1.2047619047619047</v>
+        <v>1.3592592592592594</v>
       </c>
       <c r="E10">
-        <v>1.2833333333333332</v>
+        <v>0.97500000000000009</v>
       </c>
       <c r="F10">
-        <v>1.1916666666666669</v>
+        <v>1.4690476190476189</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -757,16 +757,16 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1.5155555555555558</v>
+        <v>1.1983333333333333</v>
       </c>
       <c r="E11">
-        <v>0.72777777777777786</v>
+        <v>0.64583333333333359</v>
       </c>
       <c r="F11">
-        <v>1.7125000000000004</v>
+        <v>1.5666666666666664</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,16 +777,16 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>0.75833333333333341</v>
+        <v>1.5711111111111109</v>
       </c>
       <c r="E12">
-        <v>0.67222222222222205</v>
+        <v>0.50833333333333275</v>
       </c>
       <c r="F12">
-        <v>0.79523809523809541</v>
+        <v>1.7346153846153844</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,16 +794,19 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>1.8294871794871796</v>
+        <v>1.3589743589743588</v>
+      </c>
+      <c r="E13">
+        <v>0.61666666666666625</v>
       </c>
       <c r="F13">
-        <v>1.8294871794871796</v>
+        <v>1.4208333333333332</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,19 +814,19 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1.5633333333333332</v>
+        <v>0.7333333333333335</v>
       </c>
       <c r="E14">
-        <v>0.26666666666666661</v>
+        <v>0.51333333333333353</v>
       </c>
       <c r="F14">
-        <v>1.7074074074074075</v>
+        <v>0.91666666666666685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>